<commit_message>
check the presence of structures + HU value + volume value
</commit_message>
<xml_diff>
--- a/Plancheck/protocol_check/prostate.xlsx
+++ b/Plancheck/protocol_check/prostate.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="opt structures" sheetId="3" r:id="rId3"/>
     <sheet name="couch_structures" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -231,19 +231,25 @@
     <t>CouchSurface</t>
   </si>
   <si>
-    <t>zzExt_Orfit</t>
-  </si>
-  <si>
-    <t>zzInt_Orfit</t>
-  </si>
-  <si>
     <t>HU</t>
+  </si>
+  <si>
+    <t>zzInt_ORFIT</t>
+  </si>
+  <si>
+    <t>zzExt_ORFIT</t>
+  </si>
+  <si>
+    <t>vol min</t>
+  </si>
+  <si>
+    <t>vol max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -764,10 +770,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,119 +781,137 @@
     <col min="1" max="1" width="16.42578125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -901,10 +925,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,82 +936,91 @@
     <col min="1" max="1" width="28.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
@@ -1062,10 +1095,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,15 +1106,21 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>67</v>
       </c>
@@ -1089,7 +1128,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
@@ -1097,15 +1136,15 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
check if excel cell is empty
</commit_message>
<xml_diff>
--- a/Plancheck/protocol_check/prostate.xlsx
+++ b/Plancheck/protocol_check/prostate.xlsx
@@ -250,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,8 +281,112 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,8 +417,181 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -322,11 +599,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -350,9 +775,52 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -770,10 +1238,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +1249,7 @@
     <col min="1" max="1" width="16.42578125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -795,123 +1263,222 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="14">
+        <v>112.02</v>
+      </c>
+      <c r="D10" s="14">
+        <v>5569.9416345124491</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="14">
+        <v>39.14</v>
+      </c>
+      <c r="D15" s="14">
+        <v>560.73982355024589</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17">
-        <v>30</v>
-      </c>
-      <c r="D17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="14">
+        <v>30.94</v>
+      </c>
+      <c r="D17" s="14">
+        <v>130.38317839653934</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="14">
+        <v>9.1</v>
+      </c>
+      <c r="D19" s="14">
+        <v>309.59451169159098</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="14">
+        <v>96.808165954476038</v>
+      </c>
+      <c r="D20" s="14">
+        <v>270.90074153704302</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="14">
+        <v>100.38</v>
+      </c>
+      <c r="D21" s="14">
+        <v>271.54249032790631</v>
+      </c>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B23">
         <v>0</v>
+      </c>
+      <c r="C23" s="14">
+        <v>91.37</v>
+      </c>
+      <c r="D23" s="14">
+        <v>581.80274094704828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>